<commit_message>
Update the new methods
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/RestAssuredDataDriven.xlsx
+++ b/src/test/resources/TestData/RestAssuredDataDriven.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESoft_Solutions\API_Testing\RestAssured_DataDriven\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688A0DF5-6DAF-40DA-AA6A-2C8F9FA97C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254B68D0-BDE7-4A3C-8235-140299DCDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Headers</t>
   </si>
@@ -85,6 +85,18 @@
   "last_login": "$RandomPastDate",
   "email_verified": "$RandomBooleanValue"
 }</t>
+  </si>
+  <si>
+    <t>QueryParameters</t>
+  </si>
+  <si>
+    <t>name=happy, priya=nothing</t>
+  </si>
+  <si>
+    <t>name=new, priya=nothing</t>
+  </si>
+  <si>
+    <t>users/1/{name}/{priya}</t>
   </si>
 </sst>
 </file>
@@ -455,24 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5541BD12-A439-4E4D-A885-95CACA3FF36F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1" collapsed="1"/>
+    <col min="3" max="3" width="14.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="39.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -480,80 +493,97 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>